<commit_message>
纠正 flag[16] [17] 范围错误
</commit_message>
<xml_diff>
--- a/flags.xlsx
+++ b/flags.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Others\Github\deltarune-studies\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D074231-6086-4850-8A09-657CF0E793A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="23655" windowHeight="9570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>行号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,12 +108,6 @@
   <si>
     <t>0&lt;=float&lt;=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0&lt;=float&lt;=2</t>
-  </si>
-  <si>
-    <t>0&lt;=float&lt;=3</t>
   </si>
   <si>
     <t>未使用</t>
@@ -484,12 +484,16 @@
     <t>是否与 room_forest_area1 房间的“蜜蜂罐”对话</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>0&lt;=float&lt;=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,11 +586,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -628,7 +640,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -660,9 +672,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,6 +724,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -869,23 +917,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="50.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="50.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -899,10 +947,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -910,10 +958,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>6</v>
       </c>
@@ -921,10 +969,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>7</v>
       </c>
@@ -932,10 +980,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>8</v>
       </c>
@@ -943,13 +991,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>9</v>
       </c>
@@ -957,10 +1005,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>10</v>
       </c>
@@ -968,10 +1016,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>11</v>
       </c>
@@ -979,10 +1027,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>12</v>
       </c>
@@ -990,13 +1038,13 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>13</v>
       </c>
@@ -1004,10 +1052,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>14</v>
       </c>
@@ -1015,10 +1063,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>15</v>
       </c>
@@ -1029,10 +1077,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>16</v>
       </c>
@@ -1040,13 +1088,13 @@
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>17</v>
       </c>
@@ -1054,40 +1102,40 @@
         <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>29</v>
       </c>
@@ -1095,24 +1143,24 @@
         <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>31</v>
       </c>
@@ -1120,10 +1168,10 @@
         <v>15</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>32</v>
       </c>
@@ -1131,40 +1179,40 @@
         <v>15</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>53</v>
       </c>
@@ -1172,21 +1220,21 @@
         <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>100</v>
       </c>
@@ -1194,32 +1242,32 @@
         <v>15</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>104</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>105</v>
       </c>
@@ -1227,10 +1275,10 @@
         <v>15</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>106</v>
       </c>
@@ -1238,18 +1286,18 @@
         <v>15</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>107</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>108</v>
       </c>
@@ -1257,18 +1305,18 @@
         <v>15</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>112</v>
       </c>
@@ -1276,18 +1324,18 @@
         <v>15</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>115</v>
       </c>
@@ -1295,18 +1343,18 @@
         <v>18</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>200</v>
       </c>
@@ -1314,13 +1362,13 @@
         <v>18</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>201</v>
       </c>
@@ -1328,24 +1376,24 @@
         <v>15</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="40.5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>202</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>203</v>
       </c>
@@ -1353,38 +1401,38 @@
         <v>17</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>204</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="67.5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="72" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>205</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>206</v>
       </c>
@@ -1392,21 +1440,21 @@
         <v>17</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>207</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>208</v>
       </c>
@@ -1414,13 +1462,13 @@
         <v>15</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>209</v>
       </c>
@@ -1428,62 +1476,62 @@
         <v>15</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="27">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>210</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>211</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>212</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>213</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>214</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="40.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>215</v>
       </c>
@@ -1491,13 +1539,13 @@
         <v>17</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>216</v>
       </c>
@@ -1505,10 +1553,10 @@
         <v>15</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>217</v>
       </c>
@@ -1516,10 +1564,10 @@
         <v>15</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>218</v>
       </c>
@@ -1527,67 +1575,67 @@
         <v>15</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>219</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>229</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>230</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>231</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>232</v>
       </c>
@@ -1595,10 +1643,10 @@
         <v>15</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>233</v>
       </c>
@@ -1606,13 +1654,13 @@
         <v>15</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>234</v>
       </c>
@@ -1625,12 +1673,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1638,12 +1686,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>